<commit_message>
Added missing results for Terence Brown Added 2 more flags for Liran and Martin
</commit_message>
<xml_diff>
--- a/data/2022-04-04/SCW Weekly Comp 2022-04-04 (Responses).xlsx
+++ b/data/2022-04-04/SCW Weekly Comp 2022-04-04 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="201">
   <si>
     <t>Timestamp</t>
   </si>
@@ -596,6 +596,24 @@
   </si>
   <si>
     <t>https://www.facebook.com/events/1171138513621623?post_id=1179781856090622&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>Terence Brown</t>
+  </si>
+  <si>
+    <t>2021BROW05</t>
+  </si>
+  <si>
+    <t>https://m.facebook.com/events/655069328915915?view=permalink&amp;id=658387461917435</t>
+  </si>
+  <si>
+    <t>https://m.facebook.com/events/655069328915915?view=permalink&amp;id=658388595250655</t>
+  </si>
+  <si>
+    <t>https://m.facebook.com/events/1171138513621623?view=permalink&amp;id=1174670813268393</t>
+  </si>
+  <si>
+    <t>https://m.facebook.com/events/1171138513621623?view=permalink&amp;id=1174672186601589</t>
   </si>
 </sst>
 </file>
@@ -3290,6 +3308,170 @@
         <v>10.54</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>44673.83113694444</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H55" s="3">
+        <v>12.24</v>
+      </c>
+      <c r="I55" s="3">
+        <v>7.07</v>
+      </c>
+      <c r="J55" s="3">
+        <v>7.85</v>
+      </c>
+      <c r="K55" s="3">
+        <v>8.03</v>
+      </c>
+      <c r="L55" s="3">
+        <v>6.74</v>
+      </c>
+      <c r="M55" s="3">
+        <v>6.74</v>
+      </c>
+      <c r="N55" s="3">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>44673.832441736115</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O56" s="3">
+        <v>29.67</v>
+      </c>
+      <c r="P56" s="3">
+        <v>18.87</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>25.05</v>
+      </c>
+      <c r="R56" s="3">
+        <v>34.2</v>
+      </c>
+      <c r="S56" s="3">
+        <v>23.39</v>
+      </c>
+      <c r="T56" s="3">
+        <v>18.87</v>
+      </c>
+      <c r="U56" s="3">
+        <v>26.04</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>44673.83392185185</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="BO57" s="3">
+        <v>10.69</v>
+      </c>
+      <c r="BP57" s="3">
+        <v>11.89</v>
+      </c>
+      <c r="BQ57" s="3">
+        <v>10.47</v>
+      </c>
+      <c r="BR57" s="3">
+        <v>13.23</v>
+      </c>
+      <c r="BS57" s="3">
+        <v>9.51</v>
+      </c>
+      <c r="BT57" s="3">
+        <v>9.51</v>
+      </c>
+      <c r="BU57" s="3">
+        <v>11.02</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>44673.835416076385</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="BV58" s="3">
+        <v>27.62</v>
+      </c>
+      <c r="BW58" s="3">
+        <v>45.94</v>
+      </c>
+      <c r="BX58" s="3">
+        <v>32.68</v>
+      </c>
+      <c r="BY58" s="3">
+        <v>34.54</v>
+      </c>
+      <c r="BZ58" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="CA58" s="3">
+        <v>27.62</v>
+      </c>
+      <c r="CB58" s="3">
+        <v>37.72</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
@@ -3345,7 +3527,11 @@
     <hyperlink r:id="rId51" ref="F52"/>
     <hyperlink r:id="rId52" ref="F53"/>
     <hyperlink r:id="rId53" ref="F54"/>
+    <hyperlink r:id="rId54" ref="F55"/>
+    <hyperlink r:id="rId55" ref="F56"/>
+    <hyperlink r:id="rId56" ref="F57"/>
+    <hyperlink r:id="rId57" ref="F58"/>
   </hyperlinks>
-  <drawing r:id="rId54"/>
+  <drawing r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>